<commit_message>
import students using excel file not csv
</commit_message>
<xml_diff>
--- a/templates/import_teachers.xlsx
+++ b/templates/import_teachers.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\srms_makumbusho\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MolapoHighSchool\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96AAF80E-737A-4215-99EB-C033CBD5C1F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>FIRST NAME</t>
   </si>
@@ -38,17 +39,29 @@
     <t>GENDER</t>
   </si>
   <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
+    <t>lesala</t>
+  </si>
+  <si>
+    <t>lesala@gmail.com</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>likobo</t>
+  </si>
+  <si>
+    <t>likobo@gmail.com</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +78,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -112,7 +133,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
@@ -428,23 +449,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="59.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -457,26 +477,46 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Male,Female"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
-      <formula1>"Active, Inactive"</formula1>
-    </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{1638E377-6EAC-4517-85A8-301ED33B9014}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{92FD0197-4FE5-4761-8ED4-6DB22DF578D4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>